<commit_message>
Adding files and making updates to framework for both POST and GET methods
</commit_message>
<xml_diff>
--- a/src/main/resources/data/ServiceTestdata.xlsx
+++ b/src/main/resources/data/ServiceTestdata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>Scenario 1</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>rahulshettyacademy.com</t>
+  </si>
+  <si>
+    <t>/maps/api/place/get/json</t>
+  </si>
+  <si>
+    <t>Scenario 2</t>
   </si>
 </sst>
 </file>
@@ -503,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -628,14 +634,54 @@
       </c>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>-38.383493999999999</v>
+      </c>
+      <c r="I3" s="1">
+        <v>33.427362000000002</v>
+      </c>
+      <c r="J3" s="1">
+        <v>50</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="1"/>
@@ -700,8 +746,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding files and making updates to framework
</commit_message>
<xml_diff>
--- a/src/main/resources/data/ServiceTestdata.xlsx
+++ b/src/main/resources/data/ServiceTestdata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
   <si>
     <t>Scenario 1</t>
   </si>
@@ -117,6 +117,21 @@
   </si>
   <si>
     <t>Scenario 2</t>
+  </si>
+  <si>
+    <t>place_id</t>
+  </si>
+  <si>
+    <t>d6790ea8c04cea36517edcec20da0212</t>
+  </si>
+  <si>
+    <t>ef6ed47dffcf1a24b70ef776662f2bc1</t>
+  </si>
+  <si>
+    <t>Scenario 3</t>
+  </si>
+  <si>
+    <t>/maps/api/place/delete/json</t>
   </si>
 </sst>
 </file>
@@ -507,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -531,9 +546,10 @@
     <col min="14" max="14" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="34.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1" ht="36.75" thickBot="1">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="36.75" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -582,8 +598,11 @@
       <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:17">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -632,8 +651,9 @@
       <c r="P2" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:17">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -682,18 +702,60 @@
       <c r="P3" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="Q3" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+    <row r="4" spans="1:17">
+      <c r="A4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4">
+        <v>-38.383493999999999</v>
+      </c>
+      <c r="I4" s="1">
+        <v>33.427362000000002</v>
+      </c>
+      <c r="J4" s="1">
+        <v>50</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:17">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -703,7 +765,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:17">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -713,7 +775,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:17">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -723,7 +785,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:17">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -733,7 +795,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:17">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -747,8 +809,9 @@
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
     <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Put Response and json values
</commit_message>
<xml_diff>
--- a/src/main/resources/data/ServiceTestdata.xlsx
+++ b/src/main/resources/data/ServiceTestdata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\308211\IdeaProjects\ccs-scale-cat-test\src\main\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\204157\Downloads\ccs-scale-cat-tests-master\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15348" windowHeight="4548"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>Scenario 1</t>
   </si>
@@ -74,9 +74,6 @@
     <t>language</t>
   </si>
   <si>
-    <t>Shoe park_shop</t>
-  </si>
-  <si>
     <t>http://google.com</t>
   </si>
   <si>
@@ -86,33 +83,6 @@
     <t>location_lng</t>
   </si>
   <si>
-    <t>Frontline House</t>
-  </si>
-  <si>
-    <t>(+91) 983 893 3937</t>
-  </si>
-  <si>
-    <t>29, side layout, cohen 09</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>Add place API call</t>
-  </si>
-  <si>
-    <t>origin</t>
-  </si>
-  <si>
-    <t>host</t>
-  </si>
-  <si>
-    <t>https://rahulshettyacademy.com</t>
-  </si>
-  <si>
-    <t>rahulshettyacademy.com</t>
-  </si>
-  <si>
     <t>/maps/api/place/get/json</t>
   </si>
   <si>
@@ -122,12 +92,6 @@
     <t>place_id</t>
   </si>
   <si>
-    <t>d6790ea8c04cea36517edcec20da0212</t>
-  </si>
-  <si>
-    <t>ef6ed47dffcf1a24b70ef776662f2bc1</t>
-  </si>
-  <si>
     <t>Scenario 3</t>
   </si>
   <si>
@@ -137,19 +101,31 @@
     <t>Scenario 4</t>
   </si>
   <si>
-    <t>Get place API call</t>
-  </si>
-  <si>
-    <t>Delete place API call</t>
-  </si>
-  <si>
-    <t>Update place API call</t>
-  </si>
-  <si>
     <t>/maps/api/place/update/json</t>
   </si>
   <si>
-    <t>(+91) 929 875 0767</t>
+    <t>msg</t>
+  </si>
+  <si>
+    <t>Address successfully updated</t>
+  </si>
+  <si>
+    <t>b2a02a18457c171a598437f197b916ec</t>
+  </si>
+  <si>
+    <t>70 Summer walk, UAE</t>
+  </si>
+  <si>
+    <t>Frontline house</t>
+  </si>
+  <si>
+    <t>(+91) 983 893 3937</t>
+  </si>
+  <si>
+    <t>29, side layout, cohen 09</t>
+  </si>
+  <si>
+    <t>Shoe park, shop</t>
   </si>
 </sst>
 </file>
@@ -540,340 +516,287 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.140625" customWidth="1"/>
-    <col min="13" max="13" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5546875" customWidth="1"/>
+    <col min="9" max="9" width="23.109375" customWidth="1"/>
+    <col min="10" max="10" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="34.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="36.75" thickBot="1">
+    <row r="1" spans="1:15" s="3" customFormat="1" ht="35.4" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>31</v>
-      </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:15">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>-38.383493999999999</v>
+      </c>
+      <c r="F2" s="1">
+        <v>33.427362000000002</v>
+      </c>
+      <c r="G2" s="1">
+        <v>50</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>-38.383493999999999</v>
+      </c>
+      <c r="F3" s="1">
+        <v>33.427362000000002</v>
+      </c>
+      <c r="G3" s="1">
+        <v>50</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>-38.383493999999999</v>
+      </c>
+      <c r="F4" s="1">
+        <v>33.427362000000002</v>
+      </c>
+      <c r="G4" s="1">
+        <v>50</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>-38.383493999999999</v>
+      </c>
+      <c r="F5" s="1">
+        <v>33.427362000000002</v>
+      </c>
+      <c r="G5" s="1">
+        <v>50</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2">
-        <v>-38.383493999999999</v>
-      </c>
-      <c r="I2" s="1">
-        <v>33.427362000000002</v>
-      </c>
-      <c r="J2" s="1">
-        <v>50</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q2" s="1"/>
+      <c r="O5" s="1"/>
     </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3">
-        <v>-38.383493999999999</v>
-      </c>
-      <c r="I3" s="1">
-        <v>33.427362000000002</v>
-      </c>
-      <c r="J3" s="1">
-        <v>50</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4">
-        <v>-38.383493999999999</v>
-      </c>
-      <c r="I4" s="1">
-        <v>33.427362000000002</v>
-      </c>
-      <c r="J4" s="1">
-        <v>50</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5">
-        <v>-38.383493999999999</v>
-      </c>
-      <c r="I5" s="1">
-        <v>33.427362000000002</v>
-      </c>
-      <c r="J5" s="1">
-        <v>50</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:15">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:15">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated methods for API capabilities
</commit_message>
<xml_diff>
--- a/src/main/resources/data/ServiceTestdata.xlsx
+++ b/src/main/resources/data/ServiceTestdata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\204157\Downloads\ccs-scale-cat-tests-master\src\main\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\308211\IdeaProjects\ccs-scale-cat-test\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15348" windowHeight="4548"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4545"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
   <si>
     <t>Scenario 1</t>
   </si>
@@ -74,6 +74,9 @@
     <t>language</t>
   </si>
   <si>
+    <t>Shoe park_shop</t>
+  </si>
+  <si>
     <t>http://google.com</t>
   </si>
   <si>
@@ -83,6 +86,33 @@
     <t>location_lng</t>
   </si>
   <si>
+    <t>Frontline House</t>
+  </si>
+  <si>
+    <t>(+91) 983 893 3937</t>
+  </si>
+  <si>
+    <t>29, side layout, cohen 09</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Add place API call</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>host</t>
+  </si>
+  <si>
+    <t>https://rahulshettyacademy.com</t>
+  </si>
+  <si>
+    <t>rahulshettyacademy.com</t>
+  </si>
+  <si>
     <t>/maps/api/place/get/json</t>
   </si>
   <si>
@@ -92,6 +122,9 @@
     <t>place_id</t>
   </si>
   <si>
+    <t>ef6ed47dffcf1a24b70ef776662f2bc1</t>
+  </si>
+  <si>
     <t>Scenario 3</t>
   </si>
   <si>
@@ -101,31 +134,22 @@
     <t>Scenario 4</t>
   </si>
   <si>
+    <t>Get place API call</t>
+  </si>
+  <si>
+    <t>Delete place API call</t>
+  </si>
+  <si>
+    <t>Update place API call</t>
+  </si>
+  <si>
     <t>/maps/api/place/update/json</t>
   </si>
   <si>
-    <t>msg</t>
-  </si>
-  <si>
-    <t>Address successfully updated</t>
-  </si>
-  <si>
-    <t>b2a02a18457c171a598437f197b916ec</t>
-  </si>
-  <si>
-    <t>70 Summer walk, UAE</t>
-  </si>
-  <si>
-    <t>Frontline house</t>
-  </si>
-  <si>
-    <t>(+91) 983 893 3937</t>
-  </si>
-  <si>
-    <t>29, side layout, cohen 09</t>
-  </si>
-  <si>
-    <t>Shoe park, shop</t>
+    <t>(+91) 929 875 0767</t>
+  </si>
+  <si>
+    <t>f8c34795029a2753ed03ac7861f43c4d</t>
   </si>
 </sst>
 </file>
@@ -516,287 +540,338 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5546875" customWidth="1"/>
-    <col min="9" max="9" width="23.109375" customWidth="1"/>
-    <col min="10" max="10" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.140625" customWidth="1"/>
+    <col min="13" max="13" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="34.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" ht="35.4" thickBot="1">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="36.75" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>26</v>
+      <c r="Q1" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:17">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2">
+      <c r="H2">
         <v>-38.383493999999999</v>
       </c>
-      <c r="F2" s="1">
+      <c r="I2" s="1">
         <v>33.427362000000002</v>
       </c>
-      <c r="G2" s="1">
+      <c r="J2" s="1">
         <v>50</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="K2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>-38.383493999999999</v>
+      </c>
+      <c r="I3" s="1">
+        <v>33.427362000000002</v>
+      </c>
+      <c r="J3" s="1">
+        <v>50</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4">
+        <v>-38.383493999999999</v>
+      </c>
+      <c r="I4" s="1">
+        <v>33.427362000000002</v>
+      </c>
+      <c r="J4" s="1">
+        <v>50</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <v>-38.383493999999999</v>
+      </c>
+      <c r="I5" s="1">
+        <v>33.427362000000002</v>
+      </c>
+      <c r="J5" s="1">
+        <v>50</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3">
-        <v>-38.383493999999999</v>
-      </c>
-      <c r="F3" s="1">
-        <v>33.427362000000002</v>
-      </c>
-      <c r="G3" s="1">
-        <v>50</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O3" s="1"/>
+    <row r="6" spans="1:17">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
     </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>-38.383493999999999</v>
-      </c>
-      <c r="F4" s="1">
-        <v>33.427362000000002</v>
-      </c>
-      <c r="G4" s="1">
-        <v>50</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5">
-        <v>-38.383493999999999</v>
-      </c>
-      <c r="F5" s="1">
-        <v>33.427362000000002</v>
-      </c>
-      <c r="G5" s="1">
-        <v>50</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O5" s="1"/>
-    </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:17">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:17">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:17">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>